<commit_message>
Period : default start date is h-1
</commit_message>
<xml_diff>
--- a/assets/images/Analisa.xlsx
+++ b/assets/images/Analisa.xlsx
@@ -15,12 +15,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>2022-05-19</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;19 Mei ada......&lt;/p&gt;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+  <si>
+    <t>2022-06-02</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Analisa tanggal 2 juni 2&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>2022-06-01</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;ASSSSSSSSSSSSSS&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>2022-05-31</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Naiknya harga BBM dsa&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Analisa tanggal 2 juni&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>2022-05-30</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ww&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Re&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lumen (8.3.4) (Laravel Components ^8.0)&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -356,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -364,15 +391,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>